<commit_message>
Playing with the Excel
</commit_message>
<xml_diff>
--- a/Working/HW1_BoxModel_Excel/Starter_Code/1D ss satd.xlsx
+++ b/Working/HW1_BoxModel_Excel/Starter_Code/1D ss satd.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laura/Documents/Teaching/Groundwater_Modeling/HWRS582_Spring22/Git_Course-Materials22/Assignments/HW1_BoxModel_Excel/Starter_Code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xy_22\Documents\MSc._Hydrology\2022_Spring\GW_Modelling\homework-xenidegracia\Working\HW1_BoxModel_Excel\Starter_Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8786C6-777E-6A42-B878-51F1B241E14F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78554480-02D8-4B29-A9F1-6D49410BABB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="760" windowWidth="29200" windowHeight="18420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs" sheetId="2" r:id="rId1"/>
     <sheet name="model and key plot" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -509,37 +509,37 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>94.592080577586103</c:v>
+                  <c:v>94.592428984586022</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>89.184522549972243</c:v>
+                  <c:v>89.185169279793001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>83.777454663358</c:v>
+                  <c:v>83.778331789428435</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>78.370961180827933</c:v>
+                  <c:v>78.371989098911868</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>72.965079023127814</c:v>
+                  <c:v>72.966173012298839</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64.856874572392442</c:v>
+                  <c:v>64.857981913281293</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>54.046518847691296</c:v>
+                  <c:v>54.047563120118134</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43.236672013469864</c:v>
+                  <c:v>43.237582692452293</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32.427228205985386</c:v>
+                  <c:v>32.427949437749994</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>21.618060202617919</c:v>
+                  <c:v>21.618553764636921</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10.809030101308959</c:v>
+                  <c:v>10.809276882318461</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -873,40 +873,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="1">
-                  <c:v>2.1631677689655588E-2</c:v>
+                  <c:v>2.1630284061655916E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.1630232110455436E-2</c:v>
+                  <c:v>2.1629038819172081E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.1628271546456971E-2</c:v>
+                  <c:v>2.1627349961458268E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.1625973930120269E-2</c:v>
+                  <c:v>2.1625370762066266E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.1623528630800477E-2</c:v>
+                  <c:v>2.1623264346452117E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.1621878535294323E-2</c:v>
+                  <c:v>2.1621842930713453E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.1620711449402294E-2</c:v>
+                  <c:v>2.1620837586326318E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.1619693668442866E-2</c:v>
+                  <c:v>2.1619960855331685E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.1618887614968954E-2</c:v>
+                  <c:v>2.1619266509404596E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.1618336006734937E-2</c:v>
+                  <c:v>2.1618791346226147E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.1618060202617917E-2</c:v>
+                  <c:v>2.1618553764636922E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.1618060202617917E-2</c:v>
+                  <c:v>2.1618553764636922E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1752,14 +1752,14 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>10</v>
       </c>
@@ -1778,13 +1778,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>13</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>1</v>
       </c>
@@ -1803,10 +1803,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>15</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>5</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>6</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>22</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>14</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D17" s="1">
         <v>1</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D18" s="1">
         <v>1</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D19" s="1">
         <v>1</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D20" s="1">
         <v>1</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D21" s="1">
         <v>1</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D22" s="1">
         <v>1</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D23" s="1">
         <v>1</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D24" s="1">
         <v>3</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D25" s="1">
         <v>3</v>
       </c>
@@ -1937,7 +1937,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D26" s="1">
         <v>3</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D27" s="1">
         <v>3</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>16</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>18</v>
       </c>
@@ -1975,17 +1975,17 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C34" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>21</v>
       </c>
@@ -2009,15 +2009,15 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="6.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.6328125" customWidth="1"/>
+    <col min="8" max="8" width="6.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:20" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="2:20" ht="14" thickTop="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:20" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:20" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="22" t="s">
         <v>32</v>
       </c>
@@ -2028,7 +2028,7 @@
       <c r="S4" s="14"/>
       <c r="T4" s="15"/>
     </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
       <c r="D5" s="5"/>
@@ -2039,7 +2039,7 @@
       <c r="S5" s="26"/>
       <c r="T5" s="27"/>
     </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="4" t="s">
         <v>12</v>
@@ -2076,7 +2076,7 @@
       <c r="S6" s="6"/>
       <c r="T6" s="17"/>
     </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>28</v>
       </c>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="T7" s="17"/>
     </row>
-    <row r="8" spans="2:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:20" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B8" s="3" t="s">
         <v>29</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:20" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="s">
         <v>30</v>
       </c>
@@ -2180,11 +2180,11 @@
       </c>
       <c r="I9" s="1">
         <f t="shared" ref="I9:I19" ca="1" si="0">(I8*2/(1/H8+1/H9)+I10*2/(1/H9+1/H10))/(2/(1/H8+1/H9)+2/(1/H9+1/H10))</f>
-        <v>94.592080577586103</v>
+        <v>94.592428984586022</v>
       </c>
       <c r="J9" s="1">
         <f ca="1">(I8-I9)/inputs!$D$8*2/(1/H8+1/H9)</f>
-        <v>2.1631677689655588E-2</v>
+        <v>2.1630284061655916E-2</v>
       </c>
       <c r="L9">
         <f t="shared" ref="L9:L20" si="1">IF($G9=1,1,0)</f>
@@ -2209,7 +2209,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:20" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B10" s="3"/>
       <c r="C10" s="6"/>
       <c r="D10" s="7"/>
@@ -2227,11 +2227,11 @@
       </c>
       <c r="I10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>89.184522549972243</v>
+        <v>89.185169279793001</v>
       </c>
       <c r="J10" s="1">
         <f ca="1">(I9-I10)/inputs!$D$8*2/(1/H9+1/H10)</f>
-        <v>2.1630232110455436E-2</v>
+        <v>2.1629038819172081E-2</v>
       </c>
       <c r="L10">
         <f t="shared" si="1"/>
@@ -2256,7 +2256,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:20" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
@@ -2279,11 +2279,11 @@
       </c>
       <c r="I11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>83.777454663358</v>
+        <v>83.778331789428435</v>
       </c>
       <c r="J11" s="1">
         <f ca="1">(I10-I11)/inputs!$D$8*2/(1/H10+1/H11)</f>
-        <v>2.1628271546456971E-2</v>
+        <v>2.1627349961458268E-2</v>
       </c>
       <c r="L11">
         <f t="shared" si="1"/>
@@ -2308,7 +2308,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="8" t="s">
         <v>7</v>
       </c>
@@ -2331,11 +2331,11 @@
       </c>
       <c r="I12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>78.370961180827933</v>
+        <v>78.371989098911868</v>
       </c>
       <c r="J12" s="1">
         <f ca="1">(I11-I12)/inputs!$D$8*2/(1/H11+1/H12)</f>
-        <v>2.1625973930120269E-2</v>
+        <v>2.1625370762066266E-2</v>
       </c>
       <c r="L12">
         <f t="shared" si="1"/>
@@ -2360,7 +2360,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="2:20" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:20" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="F13" s="1">
         <f>F14+inputs!$D$8</f>
         <v>35</v>
@@ -2375,11 +2375,11 @@
       </c>
       <c r="I13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>72.965079023127814</v>
+        <v>72.966173012298839</v>
       </c>
       <c r="J13" s="1">
         <f ca="1">(I12-I13)/inputs!$D$8*2/(1/H12+1/H13)</f>
-        <v>2.1623528630800477E-2</v>
+        <v>2.1623264346452117E-2</v>
       </c>
       <c r="L13">
         <f t="shared" si="1"/>
@@ -2404,7 +2404,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:20" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F14" s="1">
         <f>F15+inputs!$D$8</f>
         <v>30</v>
@@ -2418,11 +2418,11 @@
       </c>
       <c r="I14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>64.856874572392442</v>
+        <v>64.857981913281293</v>
       </c>
       <c r="J14" s="1">
         <f ca="1">(I13-I14)/inputs!$D$8*2/(1/H13+1/H14)</f>
-        <v>2.1621878535294323E-2</v>
+        <v>2.1621842930713453E-2</v>
       </c>
       <c r="L14">
         <f t="shared" si="1"/>
@@ -2447,7 +2447,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="2:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:20" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F15" s="1">
         <f>F16+inputs!$D$8</f>
         <v>25</v>
@@ -2461,11 +2461,11 @@
       </c>
       <c r="I15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>54.046518847691296</v>
+        <v>54.047563120118134</v>
       </c>
       <c r="J15" s="1">
         <f ca="1">(I14-I15)/inputs!$D$8*2/(1/H14+1/H15)</f>
-        <v>2.1620711449402294E-2</v>
+        <v>2.1620837586326318E-2</v>
       </c>
       <c r="L15">
         <f t="shared" si="1"/>
@@ -2490,7 +2490,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="2:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:20" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F16" s="1">
         <f>F17+inputs!$D$8</f>
         <v>20</v>
@@ -2504,11 +2504,11 @@
       </c>
       <c r="I16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43.236672013469864</v>
+        <v>43.237582692452293</v>
       </c>
       <c r="J16" s="1">
         <f ca="1">(I15-I16)/inputs!$D$8*2/(1/H15+1/H16)</f>
-        <v>2.1619693668442866E-2</v>
+        <v>2.1619960855331685E-2</v>
       </c>
       <c r="L16">
         <f t="shared" si="1"/>
@@ -2533,7 +2533,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="6:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="6:20" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F17" s="1">
         <f>F18+inputs!$D$8</f>
         <v>15</v>
@@ -2547,11 +2547,11 @@
       </c>
       <c r="I17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>32.427228205985386</v>
+        <v>32.427949437749994</v>
       </c>
       <c r="J17" s="1">
         <f ca="1">(I16-I17)/inputs!$D$8*2/(1/H16+1/H17)</f>
-        <v>2.1618887614968954E-2</v>
+        <v>2.1619266509404596E-2</v>
       </c>
       <c r="L17">
         <f t="shared" si="1"/>
@@ -2576,7 +2576,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="6:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="6:20" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F18" s="1">
         <f>F19+inputs!$D$8</f>
         <v>10</v>
@@ -2590,11 +2590,11 @@
       </c>
       <c r="I18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>21.618060202617919</v>
+        <v>21.618553764636921</v>
       </c>
       <c r="J18" s="1">
         <f ca="1">(I17-I18)/inputs!$D$8*2/(1/H17+1/H18)</f>
-        <v>2.1618336006734937E-2</v>
+        <v>2.1618791346226147E-2</v>
       </c>
       <c r="L18">
         <f t="shared" si="1"/>
@@ -2619,7 +2619,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="6:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="6:20" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F19" s="1">
         <f>F20+inputs!$D$8</f>
         <v>5</v>
@@ -2633,11 +2633,11 @@
       </c>
       <c r="I19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10.809030101308959</v>
+        <v>10.809276882318461</v>
       </c>
       <c r="J19" s="1">
         <f ca="1">(I18-I19)/inputs!$D$8*2/(1/H18+1/H19)</f>
-        <v>2.1618060202617917E-2</v>
+        <v>2.1618553764636922E-2</v>
       </c>
       <c r="L19">
         <f t="shared" si="1"/>
@@ -2662,7 +2662,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="6:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="6:20" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F20" s="1">
         <f>inputs!D9</f>
         <v>0</v>
@@ -2680,7 +2680,7 @@
       </c>
       <c r="J20" s="1">
         <f ca="1">(I19-I20)/inputs!$D$8*2/(1/H19+1/H20)</f>
-        <v>2.1618060202617917E-2</v>
+        <v>2.1618553764636922E-2</v>
       </c>
       <c r="L20">
         <f t="shared" si="1"/>
@@ -2705,7 +2705,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="6:20" x14ac:dyDescent="0.15">
+    <row r="31" spans="6:20" x14ac:dyDescent="0.25">
       <c r="P31" s="11"/>
     </row>
   </sheetData>

</xml_diff>